<commit_message>
Commit On Sep 25
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/AccountCreationDetails.xlsx
+++ b/src/test/java/testdata/AccountCreationDetails.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jines\eclipse-workspace\WalmartManagement\src\test\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3271A4F-F7EC-4427-AA75-AB08FC1DC68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25597676-B3EB-4F8C-87A2-4E7714FB996D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>firstname</t>
   </si>
@@ -33,55 +35,97 @@
     <t>lastname</t>
   </si>
   <si>
+    <t>postalcode</t>
+  </si>
+  <si>
+    <t>Pari</t>
+  </si>
+  <si>
+    <t>Zalawadia</t>
+  </si>
+  <si>
+    <t>M6L 1B4</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>Jinesh@2694</t>
+  </si>
+  <si>
+    <t>abcd_1234</t>
+  </si>
+  <si>
+    <t>new password</t>
+  </si>
+  <si>
+    <t>current password</t>
+  </si>
+  <si>
     <t>phone</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>ji</t>
-  </si>
-  <si>
-    <t>zz</t>
-  </si>
-  <si>
-    <t>abd</t>
-  </si>
-  <si>
-    <t>hh</t>
-  </si>
-  <si>
-    <t>..888</t>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>564.625uu</t>
+  </si>
+  <si>
+    <t>noone@hotmail.com</t>
+  </si>
+  <si>
+    <t>abcd12343</t>
   </si>
   <si>
     <t>Jinesh</t>
   </si>
   <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>564ihh</t>
-  </si>
-  <si>
-    <t>jin@gmail.</t>
-  </si>
-  <si>
-    <t>abcd1234</t>
-  </si>
-  <si>
-    <t>Pari</t>
-  </si>
-  <si>
-    <t>Zalawadia</t>
-  </si>
-  <si>
-    <t>par@hotmail.com</t>
-  </si>
-  <si>
-    <t>abf4546</t>
+    <t>Z@lawadia</t>
+  </si>
+  <si>
+    <t>456789ii</t>
+  </si>
+  <si>
+    <t>email@email.com</t>
+  </si>
+  <si>
+    <t>459766…</t>
+  </si>
+  <si>
+    <t>pari.patel4192@gmail.com</t>
+  </si>
+  <si>
+    <t>address line 1</t>
+  </si>
+  <si>
+    <t>city name</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>postal code</t>
+  </si>
+  <si>
+    <t>phone number</t>
+  </si>
+  <si>
+    <t>59 Bayshore drive</t>
+  </si>
+  <si>
+    <t>Ottawa</t>
+  </si>
+  <si>
+    <t>M2L 1L5</t>
   </si>
 </sst>
 </file>
@@ -412,13 +456,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -429,71 +475,206 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1234</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>123456789</v>
+        <v>6135698742</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{66B4814D-C6F8-4751-8744-E7BD91F5601C}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{3D053462-0D19-4E71-B80C-31667CB4F0D4}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{DE756F87-19FA-4AEC-847F-94917E188A6A}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{9DF44FF6-4AE9-47E8-9D93-3922D15B5608}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{EA542858-6235-4A8A-A15A-263C56FEF5C1}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{583987BD-223E-4C14-8D35-CDAC927920F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596DDFFE-7ED9-4376-8F02-9731577B316B}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{82BC18BA-514B-4A55-B5B6-8634B1E0A7A0}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{5582A3B5-C4B3-488A-B2E0-811ECDA4D335}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{A2E8F602-5B81-492D-A4BF-4348E8B33E5E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2BEEDE5-9957-46E1-940F-45F4F7E574A2}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2">
+        <v>613456789</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>